<commit_message>
Continuing updates to quantifying the useful variables in the CPS.
</commit_message>
<xml_diff>
--- a/Useful Variables from the CPS.xlsx
+++ b/Useful Variables from the CPS.xlsx
@@ -371,9 +371,6 @@
     <t>Used to create BLS published labor force statistics. Only created for the civilian noninstitutional population 16 and over. This variable was added to Microdata in January 1998.</t>
   </si>
   <si>
-    <t xml:space="preserve">This is concatentated with HRHHID to link between months. Before May 2004 this was separated into three component parts. </t>
-  </si>
-  <si>
     <t>Month in Sample</t>
   </si>
   <si>
@@ -425,9 +422,6 @@
     <t>Identifies whether the person is a child, a civilian adult, or an adult serving in the U.S. Armed Forces.</t>
   </si>
   <si>
-    <t xml:space="preserve">PRTAGE replaces PEAGE from May 2012 onwards.. Documentation PDF incorrectly claims that this was called PEAGE before Jan 2015. Actually labelled in Record Layout as PRTAGE from May 2012 onward. (Addtionally oddity: Jan-98 and Jan-03 have the variable listed as PRTAGE - all versions before Jan-98 and from May-04 to May-12 use PEAGE). Additionally, before Aug-05, the specifics of the topcoding are less clear. The valid entries for the variable go from 0:90 before Aug-05, presumably with topcoding only occurring at 90 for ages 90+. From Aug-05 onwards, ages 80-84 are topcoded to 80, and ages 85+ are topcoded to 85. </t>
-  </si>
-  <si>
     <t>GTCBSA replaces GEMSA in May 2004. Note that Metropolitan Statistical Area boundaries are updated every decade with the census, so take care in comparing places between years. The same code may refer to different metropolitan areas. Additionally, the boundaries of metropolitan areas can change over time. Compare with the mouch more stable county values.</t>
   </si>
   <si>
@@ -446,9 +440,6 @@
     <t>Nonexistant before January 2017, when certification and licensing status questions were first added to the microdata files.</t>
   </si>
   <si>
-    <t xml:space="preserve">PRDISFLG was added with an expansion of the disability questions in January 2009. </t>
-  </si>
-  <si>
     <t>PRUNEDUR</t>
   </si>
   <si>
@@ -456,6 +447,15 @@
   </si>
   <si>
     <t xml:space="preserve">Identifies the number of weeks of unemployment the person has had. Top-coded at 119 weeks, as of April 2011. (Do we ask how long it has been since start of temporary layoff or start of unemployment job search?) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRTAGE replaces PEAGE from May 2012 onwards.. Documentation PDF incorrectly claims that this was called PEAGE before Jan 2015. Actually labelled in Record Layout as PRTAGE from May 2012 onward. (Addtionally oddity: Jan-98 and Jan-03 have the variable listed as PRTAGE - all versions before Jan-98 and from May-04 to May-12 use PEAGE). Additionally, before Aug-05, the specifics of the topcoding are less clear. The valid entries for the variable go from 0:90 before Aug-05, with topcoding only occurring at 90 for ages 90+. From Aug-05 onwards, ages 80-84 are topcoded to 80, and ages 85+ are topcoded to 85. </t>
+  </si>
+  <si>
+    <t>PRDISFLG was added with an expansion of the disability questions in January 2009. There was not a comparable set of questions available in microdata prior to January 2009.</t>
+  </si>
+  <si>
+    <t>This is concatentated with HRHHID to link between months. Before May 2004 this was separated into three component parts. Details on combining these to recreate HRHHID2 are available below.</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -757,15 +766,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1051,10 +1051,10 @@
   <dimension ref="A1:X69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S24" sqref="S24"/>
+      <selection pane="bottomRight" activeCell="S66" sqref="S66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1075,25 +1075,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" s="14">
         <v>34335</v>
@@ -1235,12 +1235,12 @@
         <v>1</v>
       </c>
       <c r="S4" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -1294,13 +1294,13 @@
       <c r="R5" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S5" s="35" t="s">
-        <v>133</v>
+      <c r="S5" s="36" t="s">
+        <v>141</v>
       </c>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="19" t="s">
         <v>113</v>
       </c>
@@ -1352,7 +1352,7 @@
       <c r="R6" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S6" s="35"/>
+      <c r="S6" s="36"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1413,7 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="35" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -1467,15 +1467,15 @@
       <c r="R8" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S8" s="35" t="s">
-        <v>127</v>
+      <c r="S8" s="36" t="s">
+        <v>126</v>
       </c>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="20" t="b">
         <v>1</v>
@@ -1525,11 +1525,11 @@
       <c r="R9" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S9" s="35"/>
+      <c r="S9" s="36"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -1583,15 +1583,15 @@
       <c r="R10" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S10" s="35" t="s">
-        <v>126</v>
+      <c r="S10" s="36" t="s">
+        <v>125</v>
       </c>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="20" t="b">
         <v>1</v>
@@ -1641,11 +1641,11 @@
       <c r="R11" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S11" s="35"/>
+      <c r="S11" s="36"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -1699,15 +1699,15 @@
       <c r="R12" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S12" s="35" t="s">
-        <v>128</v>
+      <c r="S12" s="36" t="s">
+        <v>127</v>
       </c>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" s="20" t="b">
         <v>1</v>
@@ -1757,7 +1757,7 @@
       <c r="R13" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S13" s="35"/>
+      <c r="S13" s="36"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1873,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="X15" s="1"/>
     </row>
@@ -1933,12 +1933,12 @@
         <v>1</v>
       </c>
       <c r="S16" s="32" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="19" t="s">
@@ -1992,15 +1992,15 @@
       <c r="R17" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S17" s="35" t="s">
-        <v>138</v>
+      <c r="S17" s="36" t="s">
+        <v>136</v>
       </c>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C18" s="20" t="b">
         <v>1</v>
@@ -2050,7 +2050,7 @@
       <c r="R18" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S18" s="35"/>
+      <c r="S18" s="36"/>
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2312,10 +2312,10 @@
     </row>
     <row r="24" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C24" s="20" t="b">
         <v>1</v>
@@ -2366,7 +2366,7 @@
         <v>1</v>
       </c>
       <c r="S24" s="34" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="X24" s="1"/>
     </row>
@@ -2548,7 +2548,7 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -2602,13 +2602,13 @@
       <c r="R28" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S28" s="41" t="s">
+      <c r="S28" s="38" t="s">
         <v>46</v>
       </c>
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="19" t="s">
         <v>44</v>
       </c>
@@ -2660,11 +2660,11 @@
       <c r="R29" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S29" s="41"/>
+      <c r="S29" s="38"/>
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="19" t="s">
         <v>45</v>
       </c>
@@ -2716,11 +2716,11 @@
       <c r="R30" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S30" s="41"/>
+      <c r="S30" s="38"/>
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="39" t="s">
         <v>47</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2774,13 +2774,13 @@
       <c r="R31" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S31" s="41" t="s">
+      <c r="S31" s="38" t="s">
         <v>51</v>
       </c>
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="19" t="s">
         <v>49</v>
       </c>
@@ -2832,11 +2832,11 @@
       <c r="R32" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S32" s="41"/>
+      <c r="S32" s="38"/>
       <c r="X32" s="1"/>
     </row>
     <row r="33" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="19" t="s">
         <v>50</v>
       </c>
@@ -2888,11 +2888,11 @@
       <c r="R33" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S33" s="41"/>
+      <c r="S33" s="38"/>
       <c r="X33" s="1"/>
     </row>
     <row r="34" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="39" t="s">
         <v>52</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -2946,13 +2946,13 @@
       <c r="R34" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S34" s="41" t="s">
+      <c r="S34" s="38" t="s">
         <v>74</v>
       </c>
       <c r="X34" s="1"/>
     </row>
     <row r="35" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36"/>
+      <c r="A35" s="39"/>
       <c r="B35" s="19" t="s">
         <v>54</v>
       </c>
@@ -3004,11 +3004,11 @@
       <c r="R35" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S35" s="41"/>
+      <c r="S35" s="38"/>
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="19" t="s">
         <v>55</v>
       </c>
@@ -3060,11 +3060,11 @@
       <c r="R36" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S36" s="41"/>
+      <c r="S36" s="38"/>
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="19" t="s">
         <v>56</v>
       </c>
@@ -3116,11 +3116,11 @@
       <c r="R37" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S37" s="41"/>
+      <c r="S37" s="38"/>
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="19" t="s">
@@ -3174,13 +3174,13 @@
       <c r="R38" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S38" s="41" t="s">
+      <c r="S38" s="38" t="s">
         <v>61</v>
       </c>
       <c r="X38" s="7"/>
     </row>
     <row r="39" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
+      <c r="A39" s="39"/>
       <c r="B39" s="19" t="s">
         <v>59</v>
       </c>
@@ -3232,11 +3232,11 @@
       <c r="R39" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S39" s="41"/>
+      <c r="S39" s="38"/>
       <c r="X39" s="7"/>
     </row>
     <row r="40" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="19" t="s">
         <v>60</v>
       </c>
@@ -3288,11 +3288,11 @@
       <c r="R40" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S40" s="41"/>
+      <c r="S40" s="38"/>
       <c r="X40" s="7"/>
     </row>
     <row r="41" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="39" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="19" t="s">
@@ -3346,13 +3346,13 @@
       <c r="R41" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S41" s="41" t="s">
+      <c r="S41" s="38" t="s">
         <v>75</v>
       </c>
       <c r="X41" s="7"/>
     </row>
     <row r="42" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="36"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="19" t="s">
         <v>64</v>
       </c>
@@ -3404,11 +3404,11 @@
       <c r="R42" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S42" s="41"/>
+      <c r="S42" s="38"/>
       <c r="X42" s="7"/>
     </row>
     <row r="43" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="36"/>
+      <c r="A43" s="39"/>
       <c r="B43" s="19" t="s">
         <v>65</v>
       </c>
@@ -3460,11 +3460,11 @@
       <c r="R43" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S43" s="41"/>
+      <c r="S43" s="38"/>
       <c r="X43" s="7"/>
     </row>
     <row r="44" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="23" t="s">
         <v>66</v>
       </c>
@@ -3516,7 +3516,7 @@
       <c r="R44" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="S44" s="41"/>
+      <c r="S44" s="38"/>
       <c r="X44" s="7"/>
     </row>
     <row r="45" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3600,7 +3600,7 @@
       <c r="X46" s="7"/>
     </row>
     <row r="47" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="39" t="s">
         <v>70</v>
       </c>
       <c r="B47" s="28" t="s">
@@ -3654,15 +3654,15 @@
       <c r="R47" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S47" s="35" t="s">
-        <v>134</v>
+      <c r="S47" s="36" t="s">
+        <v>132</v>
       </c>
       <c r="X47" s="7"/>
     </row>
     <row r="48" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C48" s="21" t="b">
         <v>1</v>
@@ -3712,11 +3712,11 @@
       <c r="R48" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S48" s="35"/>
+      <c r="S48" s="36"/>
       <c r="X48" s="7"/>
     </row>
     <row r="49" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="41" t="s">
         <v>72</v>
       </c>
       <c r="B49" s="29" t="s">
@@ -3770,15 +3770,15 @@
       <c r="R49" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S49" s="35" t="s">
-        <v>135</v>
+      <c r="S49" s="36" t="s">
+        <v>133</v>
       </c>
       <c r="X49" s="1"/>
     </row>
     <row r="50" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
+      <c r="A50" s="42"/>
       <c r="B50" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C50" s="25" t="b">
         <v>0</v>
@@ -3828,7 +3828,7 @@
       <c r="R50" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="S50" s="35"/>
+      <c r="S50" s="36"/>
       <c r="X50" s="1"/>
     </row>
     <row r="51" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3970,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X53" s="1"/>
     </row>
@@ -4089,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="S55" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4348,7 +4348,7 @@
       </c>
     </row>
     <row r="61" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="36" t="s">
+      <c r="A61" s="39" t="s">
         <v>98</v>
       </c>
       <c r="B61" s="19" t="s">
@@ -4402,12 +4402,12 @@
       <c r="R61" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S61" s="35" t="s">
-        <v>136</v>
+      <c r="S61" s="36" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="36"/>
+      <c r="A62" s="39"/>
       <c r="B62" s="19" t="s">
         <v>107</v>
       </c>
@@ -4459,14 +4459,14 @@
       <c r="R62" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S62" s="35"/>
+      <c r="S62" s="36"/>
     </row>
     <row r="63" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>117</v>
       </c>
       <c r="C63" s="20" t="b">
         <v>1</v>
@@ -4632,11 +4632,11 @@
         <v>1</v>
       </c>
       <c r="S65" s="32" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="39" t="s">
         <v>109</v>
       </c>
       <c r="B66" s="19" t="s">
@@ -4691,11 +4691,11 @@
         <v>0</v>
       </c>
       <c r="S66" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="36"/>
+      <c r="A67" s="39"/>
       <c r="B67" s="19" t="s">
         <v>111</v>
       </c>
@@ -4748,11 +4748,11 @@
         <v>0</v>
       </c>
       <c r="S67" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="36"/>
+      <c r="A68" s="39"/>
       <c r="B68" s="19" t="s">
         <v>112</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="S68" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4866,6 +4866,27 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="S47:S48"/>
+    <mergeCell ref="S49:S50"/>
+    <mergeCell ref="S61:S62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="S41:S44"/>
+    <mergeCell ref="S38:S40"/>
+    <mergeCell ref="S34:S37"/>
+    <mergeCell ref="S31:S33"/>
+    <mergeCell ref="S28:S30"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="S12:S13"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
@@ -4873,27 +4894,6 @@
     <mergeCell ref="S5:S6"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="S10:S11"/>
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="S41:S44"/>
-    <mergeCell ref="S38:S40"/>
-    <mergeCell ref="S34:S37"/>
-    <mergeCell ref="S31:S33"/>
-    <mergeCell ref="S28:S30"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="S12:S13"/>
-    <mergeCell ref="S47:S48"/>
-    <mergeCell ref="S49:S50"/>
-    <mergeCell ref="S61:S62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the Useful Variables excel sheet with info on the household id.
</commit_message>
<xml_diff>
--- a/Useful Variables from the CPS.xlsx
+++ b/Useful Variables from the CPS.xlsx
@@ -344,9 +344,6 @@
     <t>PULINENO</t>
   </si>
   <si>
-    <t>This is concatentated with the HRHHID2 to link between months.</t>
-  </si>
-  <si>
     <t>HRYEAR</t>
   </si>
   <si>
@@ -456,6 +453,9 @@
   </si>
   <si>
     <t>This is concatentated with HRHHID to link between months. Before May 2004 this was separated into three component parts. Details on combining these to recreate HRHHID2 are available below.</t>
+  </si>
+  <si>
+    <t>This is concatentated with the HRHHID2 to link between months.. Before September 1995, the identifier was only 12 digits, while from Sep-95 onwards, the identifier is 15 digits. Due to various complications, it is not possible to link households month-to-month from April 1994 to August 1995.</t>
   </si>
 </sst>
 </file>
@@ -744,20 +744,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -767,6 +761,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,10 +1051,10 @@
   <dimension ref="A1:X69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S66" sqref="S66"/>
+      <selection pane="bottomRight" activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1075,25 +1075,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
+      <c r="B1" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" s="14">
         <v>34335</v>
@@ -1235,12 +1235,12 @@
         <v>1</v>
       </c>
       <c r="S4" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -1294,15 +1294,15 @@
       <c r="R5" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S5" s="36" t="s">
-        <v>141</v>
+      <c r="S5" s="37" t="s">
+        <v>140</v>
       </c>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="20" t="b">
         <v>1</v>
@@ -1352,7 +1352,7 @@
       <c r="R6" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S6" s="36"/>
+      <c r="S6" s="37"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1413,7 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -1467,15 +1467,15 @@
       <c r="R8" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S8" s="36" t="s">
-        <v>126</v>
+      <c r="S8" s="37" t="s">
+        <v>125</v>
       </c>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="20" t="b">
         <v>1</v>
@@ -1525,11 +1525,11 @@
       <c r="R9" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S9" s="36"/>
+      <c r="S9" s="37"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -1583,15 +1583,15 @@
       <c r="R10" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S10" s="36" t="s">
-        <v>125</v>
+      <c r="S10" s="37" t="s">
+        <v>124</v>
       </c>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" s="20" t="b">
         <v>1</v>
@@ -1641,11 +1641,11 @@
       <c r="R11" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S11" s="36"/>
+      <c r="S11" s="37"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -1699,15 +1699,15 @@
       <c r="R12" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S12" s="36" t="s">
-        <v>127</v>
+      <c r="S12" s="37" t="s">
+        <v>126</v>
       </c>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="20" t="b">
         <v>1</v>
@@ -1757,7 +1757,7 @@
       <c r="R13" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S13" s="36"/>
+      <c r="S13" s="37"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1873,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="X15" s="1"/>
     </row>
@@ -1933,12 +1933,12 @@
         <v>1</v>
       </c>
       <c r="S16" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="19" t="s">
@@ -1992,15 +1992,15 @@
       <c r="R17" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S17" s="36" t="s">
-        <v>136</v>
+      <c r="S17" s="37" t="s">
+        <v>135</v>
       </c>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" s="20" t="b">
         <v>1</v>
@@ -2050,7 +2050,7 @@
       <c r="R18" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S18" s="36"/>
+      <c r="S18" s="37"/>
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2312,61 +2312,61 @@
     </row>
     <row r="24" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="R24" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="S24" s="34" t="s">
         <v>139</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="P24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="R24" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="S24" s="34" t="s">
-        <v>140</v>
       </c>
       <c r="X24" s="1"/>
     </row>
@@ -2548,7 +2548,7 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="35" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -2602,13 +2602,13 @@
       <c r="R28" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S28" s="38" t="s">
+      <c r="S28" s="42" t="s">
         <v>46</v>
       </c>
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="19" t="s">
         <v>44</v>
       </c>
@@ -2660,11 +2660,11 @@
       <c r="R29" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S29" s="38"/>
+      <c r="S29" s="42"/>
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="19" t="s">
         <v>45</v>
       </c>
@@ -2716,11 +2716,11 @@
       <c r="R30" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S30" s="38"/>
+      <c r="S30" s="42"/>
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="35" t="s">
         <v>47</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2774,13 +2774,13 @@
       <c r="R31" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S31" s="38" t="s">
+      <c r="S31" s="42" t="s">
         <v>51</v>
       </c>
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="19" t="s">
         <v>49</v>
       </c>
@@ -2832,11 +2832,11 @@
       <c r="R32" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S32" s="38"/>
+      <c r="S32" s="42"/>
       <c r="X32" s="1"/>
     </row>
     <row r="33" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="19" t="s">
         <v>50</v>
       </c>
@@ -2888,11 +2888,11 @@
       <c r="R33" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S33" s="38"/>
+      <c r="S33" s="42"/>
       <c r="X33" s="1"/>
     </row>
     <row r="34" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="35" t="s">
         <v>52</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -2946,13 +2946,13 @@
       <c r="R34" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S34" s="38" t="s">
+      <c r="S34" s="42" t="s">
         <v>74</v>
       </c>
       <c r="X34" s="1"/>
     </row>
     <row r="35" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="39"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="19" t="s">
         <v>54</v>
       </c>
@@ -3004,11 +3004,11 @@
       <c r="R35" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S35" s="38"/>
+      <c r="S35" s="42"/>
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="39"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="19" t="s">
         <v>55</v>
       </c>
@@ -3060,11 +3060,11 @@
       <c r="R36" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S36" s="38"/>
+      <c r="S36" s="42"/>
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="19" t="s">
         <v>56</v>
       </c>
@@ -3116,11 +3116,11 @@
       <c r="R37" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S37" s="38"/>
+      <c r="S37" s="42"/>
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="19" t="s">
@@ -3174,13 +3174,13 @@
       <c r="R38" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S38" s="38" t="s">
+      <c r="S38" s="42" t="s">
         <v>61</v>
       </c>
       <c r="X38" s="7"/>
     </row>
     <row r="39" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="39"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="19" t="s">
         <v>59</v>
       </c>
@@ -3232,11 +3232,11 @@
       <c r="R39" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S39" s="38"/>
+      <c r="S39" s="42"/>
       <c r="X39" s="7"/>
     </row>
     <row r="40" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="39"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="19" t="s">
         <v>60</v>
       </c>
@@ -3288,11 +3288,11 @@
       <c r="R40" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S40" s="38"/>
+      <c r="S40" s="42"/>
       <c r="X40" s="7"/>
     </row>
     <row r="41" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="19" t="s">
@@ -3346,13 +3346,13 @@
       <c r="R41" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S41" s="38" t="s">
+      <c r="S41" s="42" t="s">
         <v>75</v>
       </c>
       <c r="X41" s="7"/>
     </row>
     <row r="42" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="19" t="s">
         <v>64</v>
       </c>
@@ -3404,11 +3404,11 @@
       <c r="R42" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S42" s="38"/>
+      <c r="S42" s="42"/>
       <c r="X42" s="7"/>
     </row>
     <row r="43" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
+      <c r="A43" s="35"/>
       <c r="B43" s="19" t="s">
         <v>65</v>
       </c>
@@ -3460,11 +3460,11 @@
       <c r="R43" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S43" s="38"/>
+      <c r="S43" s="42"/>
       <c r="X43" s="7"/>
     </row>
     <row r="44" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="40"/>
+      <c r="A44" s="38"/>
       <c r="B44" s="23" t="s">
         <v>66</v>
       </c>
@@ -3516,7 +3516,7 @@
       <c r="R44" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="S44" s="38"/>
+      <c r="S44" s="42"/>
       <c r="X44" s="7"/>
     </row>
     <row r="45" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3600,7 +3600,7 @@
       <c r="X46" s="7"/>
     </row>
     <row r="47" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="35" t="s">
         <v>70</v>
       </c>
       <c r="B47" s="28" t="s">
@@ -3654,15 +3654,15 @@
       <c r="R47" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S47" s="36" t="s">
-        <v>132</v>
+      <c r="S47" s="37" t="s">
+        <v>131</v>
       </c>
       <c r="X47" s="7"/>
     </row>
     <row r="48" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C48" s="21" t="b">
         <v>1</v>
@@ -3712,11 +3712,11 @@
       <c r="R48" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S48" s="36"/>
+      <c r="S48" s="37"/>
       <c r="X48" s="7"/>
     </row>
     <row r="49" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="39" t="s">
         <v>72</v>
       </c>
       <c r="B49" s="29" t="s">
@@ -3770,15 +3770,15 @@
       <c r="R49" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S49" s="36" t="s">
-        <v>133</v>
+      <c r="S49" s="37" t="s">
+        <v>132</v>
       </c>
       <c r="X49" s="1"/>
     </row>
     <row r="50" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="42"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C50" s="25" t="b">
         <v>0</v>
@@ -3828,7 +3828,7 @@
       <c r="R50" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="S50" s="36"/>
+      <c r="S50" s="37"/>
       <c r="X50" s="1"/>
     </row>
     <row r="51" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3970,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="X53" s="1"/>
     </row>
@@ -4089,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="S55" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4207,7 +4207,7 @@
         <v>1</v>
       </c>
       <c r="S57" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4348,7 +4348,7 @@
       </c>
     </row>
     <row r="61" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="35" t="s">
         <v>98</v>
       </c>
       <c r="B61" s="19" t="s">
@@ -4402,14 +4402,14 @@
       <c r="R61" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S61" s="36" t="s">
-        <v>134</v>
+      <c r="S61" s="37" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C62" s="20" t="b">
         <v>1</v>
@@ -4459,14 +4459,14 @@
       <c r="R62" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S62" s="36"/>
+      <c r="S62" s="37"/>
     </row>
     <row r="63" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="C63" s="20" t="b">
         <v>1</v>
@@ -4573,7 +4573,7 @@
         <v>1</v>
       </c>
       <c r="S64" s="32" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4632,180 +4632,180 @@
         <v>1</v>
       </c>
       <c r="S65" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="39" t="s">
+      <c r="A66" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="C66" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="P66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="R66" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S66" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="35"/>
+      <c r="B67" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C66" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D66" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G66" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H66" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="P66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q66" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="R66" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="S66" s="32" t="s">
+      <c r="C67" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G67" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="P67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="R67" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S67" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="35"/>
+      <c r="B68" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G68" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="P68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="R68" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S68" s="32" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
-      <c r="B67" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C67" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D67" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G67" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H67" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="P67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="R67" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="S67" s="32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="39"/>
-      <c r="B68" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C68" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D68" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G68" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H68" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="P68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q68" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="R68" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="S68" s="32" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4866,19 +4866,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="S47:S48"/>
-    <mergeCell ref="S49:S50"/>
-    <mergeCell ref="S61:S62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="S10:S11"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="S41:S44"/>
     <mergeCell ref="S38:S40"/>
@@ -4887,13 +4881,19 @@
     <mergeCell ref="S28:S30"/>
     <mergeCell ref="S17:S18"/>
     <mergeCell ref="S12:S13"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="S47:S48"/>
+    <mergeCell ref="S49:S50"/>
+    <mergeCell ref="S61:S62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A31:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Worked on May 2004 formatting functions. Adjusted the DataDictionaryFilesFromStata.xlsx file to assist with that process.
</commit_message>
<xml_diff>
--- a/Useful Variables from the CPS.xlsx
+++ b/Useful Variables from the CPS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12048"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -744,14 +744,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -761,12 +767,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,49 +1051,49 @@
   <dimension ref="A1:X69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S65" sqref="S65"/>
+      <selection pane="bottomRight" activeCell="I48" sqref="I48:R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="7.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="7.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="6.83203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="31" customWidth="1"/>
+    <col min="3" max="5" width="7.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="7.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="6.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="163" style="32" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1240,7 +1240,7 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -1294,13 +1294,13 @@
       <c r="R5" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S5" s="37" t="s">
+      <c r="S5" s="36" t="s">
         <v>140</v>
       </c>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="19" t="s">
         <v>112</v>
       </c>
@@ -1352,7 +1352,7 @@
       <c r="R6" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S6" s="37"/>
+      <c r="S6" s="36"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1413,7 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -1467,13 +1467,13 @@
       <c r="R8" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S8" s="37" t="s">
+      <c r="S8" s="36" t="s">
         <v>125</v>
       </c>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="19" t="s">
         <v>123</v>
       </c>
@@ -1525,11 +1525,11 @@
       <c r="R9" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S9" s="37"/>
+      <c r="S9" s="36"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -1583,13 +1583,13 @@
       <c r="R10" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S10" s="37" t="s">
+      <c r="S10" s="36" t="s">
         <v>124</v>
       </c>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="19" t="s">
         <v>121</v>
       </c>
@@ -1641,11 +1641,11 @@
       <c r="R11" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S11" s="37"/>
+      <c r="S11" s="36"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -1699,13 +1699,13 @@
       <c r="R12" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S12" s="37" t="s">
+      <c r="S12" s="36" t="s">
         <v>126</v>
       </c>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="19" t="s">
         <v>122</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="R13" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S13" s="37"/>
+      <c r="S13" s="36"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1938,7 +1938,7 @@
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="19" t="s">
@@ -1992,13 +1992,13 @@
       <c r="R17" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S17" s="37" t="s">
+      <c r="S17" s="36" t="s">
         <v>135</v>
       </c>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="19" t="s">
         <v>134</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="R18" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S18" s="37"/>
+      <c r="S18" s="36"/>
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2548,7 +2548,7 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -2602,13 +2602,13 @@
       <c r="R28" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S28" s="42" t="s">
+      <c r="S28" s="38" t="s">
         <v>46</v>
       </c>
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="19" t="s">
         <v>44</v>
       </c>
@@ -2660,11 +2660,11 @@
       <c r="R29" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S29" s="42"/>
+      <c r="S29" s="38"/>
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="19" t="s">
         <v>45</v>
       </c>
@@ -2716,11 +2716,11 @@
       <c r="R30" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S30" s="42"/>
+      <c r="S30" s="38"/>
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="39" t="s">
         <v>47</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2774,13 +2774,13 @@
       <c r="R31" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S31" s="42" t="s">
+      <c r="S31" s="38" t="s">
         <v>51</v>
       </c>
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="35"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="19" t="s">
         <v>49</v>
       </c>
@@ -2832,11 +2832,11 @@
       <c r="R32" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S32" s="42"/>
+      <c r="S32" s="38"/>
       <c r="X32" s="1"/>
     </row>
     <row r="33" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="35"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="19" t="s">
         <v>50</v>
       </c>
@@ -2888,11 +2888,11 @@
       <c r="R33" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S33" s="42"/>
+      <c r="S33" s="38"/>
       <c r="X33" s="1"/>
     </row>
     <row r="34" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="39" t="s">
         <v>52</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -2946,13 +2946,13 @@
       <c r="R34" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S34" s="42" t="s">
+      <c r="S34" s="38" t="s">
         <v>74</v>
       </c>
       <c r="X34" s="1"/>
     </row>
     <row r="35" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="35"/>
+      <c r="A35" s="39"/>
       <c r="B35" s="19" t="s">
         <v>54</v>
       </c>
@@ -3004,11 +3004,11 @@
       <c r="R35" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S35" s="42"/>
+      <c r="S35" s="38"/>
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="35"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="19" t="s">
         <v>55</v>
       </c>
@@ -3060,11 +3060,11 @@
       <c r="R36" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S36" s="42"/>
+      <c r="S36" s="38"/>
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="35"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="19" t="s">
         <v>56</v>
       </c>
@@ -3116,11 +3116,11 @@
       <c r="R37" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S37" s="42"/>
+      <c r="S37" s="38"/>
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="19" t="s">
@@ -3174,13 +3174,13 @@
       <c r="R38" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S38" s="42" t="s">
+      <c r="S38" s="38" t="s">
         <v>61</v>
       </c>
       <c r="X38" s="7"/>
     </row>
     <row r="39" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="35"/>
+      <c r="A39" s="39"/>
       <c r="B39" s="19" t="s">
         <v>59</v>
       </c>
@@ -3232,11 +3232,11 @@
       <c r="R39" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S39" s="42"/>
+      <c r="S39" s="38"/>
       <c r="X39" s="7"/>
     </row>
     <row r="40" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="35"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="19" t="s">
         <v>60</v>
       </c>
@@ -3288,11 +3288,11 @@
       <c r="R40" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S40" s="42"/>
+      <c r="S40" s="38"/>
       <c r="X40" s="7"/>
     </row>
     <row r="41" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="39" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="19" t="s">
@@ -3346,13 +3346,13 @@
       <c r="R41" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S41" s="42" t="s">
+      <c r="S41" s="38" t="s">
         <v>75</v>
       </c>
       <c r="X41" s="7"/>
     </row>
     <row r="42" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="35"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="19" t="s">
         <v>64</v>
       </c>
@@ -3404,11 +3404,11 @@
       <c r="R42" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S42" s="42"/>
+      <c r="S42" s="38"/>
       <c r="X42" s="7"/>
     </row>
     <row r="43" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="35"/>
+      <c r="A43" s="39"/>
       <c r="B43" s="19" t="s">
         <v>65</v>
       </c>
@@ -3460,11 +3460,11 @@
       <c r="R43" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S43" s="42"/>
+      <c r="S43" s="38"/>
       <c r="X43" s="7"/>
     </row>
     <row r="44" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="38"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="23" t="s">
         <v>66</v>
       </c>
@@ -3516,7 +3516,7 @@
       <c r="R44" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="S44" s="42"/>
+      <c r="S44" s="38"/>
       <c r="X44" s="7"/>
     </row>
     <row r="45" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3600,7 +3600,7 @@
       <c r="X46" s="7"/>
     </row>
     <row r="47" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="39" t="s">
         <v>70</v>
       </c>
       <c r="B47" s="28" t="s">
@@ -3654,13 +3654,13 @@
       <c r="R47" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S47" s="37" t="s">
+      <c r="S47" s="36" t="s">
         <v>131</v>
       </c>
       <c r="X47" s="7"/>
     </row>
     <row r="48" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="35"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="29" t="s">
         <v>120</v>
       </c>
@@ -3712,11 +3712,11 @@
       <c r="R48" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S48" s="37"/>
+      <c r="S48" s="36"/>
       <c r="X48" s="7"/>
     </row>
     <row r="49" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="41" t="s">
         <v>72</v>
       </c>
       <c r="B49" s="29" t="s">
@@ -3770,13 +3770,13 @@
       <c r="R49" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S49" s="37" t="s">
+      <c r="S49" s="36" t="s">
         <v>132</v>
       </c>
       <c r="X49" s="1"/>
     </row>
     <row r="50" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="40"/>
+      <c r="A50" s="42"/>
       <c r="B50" s="24" t="s">
         <v>119</v>
       </c>
@@ -3828,7 +3828,7 @@
       <c r="R50" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="S50" s="37"/>
+      <c r="S50" s="36"/>
       <c r="X50" s="1"/>
     </row>
     <row r="51" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4348,7 +4348,7 @@
       </c>
     </row>
     <row r="61" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="39" t="s">
         <v>98</v>
       </c>
       <c r="B61" s="19" t="s">
@@ -4402,12 +4402,12 @@
       <c r="R61" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="S61" s="37" t="s">
+      <c r="S61" s="36" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="35"/>
+      <c r="A62" s="39"/>
       <c r="B62" s="19" t="s">
         <v>106</v>
       </c>
@@ -4459,7 +4459,7 @@
       <c r="R62" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="S62" s="37"/>
+      <c r="S62" s="36"/>
     </row>
     <row r="63" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
@@ -4636,7 +4636,7 @@
       </c>
     </row>
     <row r="66" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="39" t="s">
         <v>108</v>
       </c>
       <c r="B66" s="19" t="s">
@@ -4695,7 +4695,7 @@
       </c>
     </row>
     <row r="67" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
+      <c r="A67" s="39"/>
       <c r="B67" s="19" t="s">
         <v>110</v>
       </c>
@@ -4752,7 +4752,7 @@
       </c>
     </row>
     <row r="68" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="35"/>
+      <c r="A68" s="39"/>
       <c r="B68" s="19" t="s">
         <v>111</v>
       </c>
@@ -4866,13 +4866,19 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="S47:S48"/>
+    <mergeCell ref="S49:S50"/>
+    <mergeCell ref="S61:S62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A48"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="S41:S44"/>
     <mergeCell ref="S38:S40"/>
@@ -4881,19 +4887,13 @@
     <mergeCell ref="S28:S30"/>
     <mergeCell ref="S17:S18"/>
     <mergeCell ref="S12:S13"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="S47:S48"/>
-    <mergeCell ref="S49:S50"/>
-    <mergeCell ref="S61:S62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="S10:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>